<commit_message>
Some updates of IE list
</commit_message>
<xml_diff>
--- a/RQ1-InformationElement/ie_verification-Ellis+xmk 0.7.xlsx
+++ b/RQ1-InformationElement/ie_verification-Ellis+xmk 0.7.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\XMK23\Dropbox\York\EMSE2020\ie_verification\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\XMK23\Dropbox\York\EMSE2020\ie_verification\收录到replication package的\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D86920F9-42E7-49F5-9FEB-35F32CEFBB17}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3E0C808-294F-49B3-A64F-DC66FC98F0C7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="350" windowWidth="19420" windowHeight="10560" xr2:uid="{C1A024D0-E93C-47C8-B91A-BC4AE02A7551}"/>
+    <workbookView xWindow="-25320" yWindow="-8490" windowWidth="25440" windowHeight="15540" xr2:uid="{C1A024D0-E93C-47C8-B91A-BC4AE02A7551}"/>
   </bookViews>
   <sheets>
     <sheet name="从第二个dimension开始校验" sheetId="3" r:id="rId1"/>
@@ -98,15 +98,9 @@
     <t>PyTorchHub</t>
   </si>
   <si>
-    <t>AIHub</t>
-  </si>
-  <si>
     <t># Download</t>
   </si>
   <si>
-    <t>Product Name</t>
-  </si>
-  <si>
     <t>PyPI</t>
   </si>
   <si>
@@ -146,9 +140,6 @@
     <t>Helpful links</t>
   </si>
   <si>
-    <t>Product Information</t>
-  </si>
-  <si>
     <t>Technical Documentation</t>
   </si>
   <si>
@@ -176,15 +167,6 @@
     <t>Extra Information</t>
   </si>
   <si>
-    <t>Product Quality Evaluation</t>
-  </si>
-  <si>
-    <t>Product Submission &amp; Repository Review</t>
-  </si>
-  <si>
-    <t>Product Component Information</t>
-  </si>
-  <si>
     <t>Information related to usage context. E.g., installation command, hardware and software environment requirements.</t>
   </si>
   <si>
@@ -197,25 +179,43 @@
     <t>Developer(s)</t>
   </si>
   <si>
-    <t xml:space="preserve">Owner, publisher or collaborators of this product. </t>
-  </si>
-  <si>
-    <t>Other information for this product, e.g., product homepage, academic references.</t>
-  </si>
-  <si>
     <t>Data Description</t>
   </si>
   <si>
     <t>Information about the dataset. E.g., dataset name, IO data shape, data pre-procession.</t>
   </si>
   <si>
-    <t>Product Domain</t>
-  </si>
-  <si>
-    <t>The application domain of the product, e.g., image classification for modules, front-end for packages.</t>
-  </si>
-  <si>
     <t>Compatibility</t>
+  </si>
+  <si>
+    <t>TFHub</t>
+  </si>
+  <si>
+    <t>Package Information</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Owner, publisher or collaborators of this Package. </t>
+  </si>
+  <si>
+    <t>Other information for this Package, e.g., Package homepage, academic references.</t>
+  </si>
+  <si>
+    <t>Package Name</t>
+  </si>
+  <si>
+    <t>Package Component Information</t>
+  </si>
+  <si>
+    <t>Package Quality Evaluation</t>
+  </si>
+  <si>
+    <t>Package Domain</t>
+  </si>
+  <si>
+    <t>The application domain of the Package, e.g., image classification for modules, front-end for packages.</t>
+  </si>
+  <si>
+    <t>Package Submission &amp; Review</t>
   </si>
 </sst>
 </file>
@@ -777,8 +777,8 @@
   <dimension ref="A1:I46"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G24" sqref="G24"/>
+      <pane ySplit="1" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A38" sqref="A38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -800,13 +800,13 @@
         <v>17</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D1" s="5" t="s">
         <v>18</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>21</v>
+        <v>51</v>
       </c>
       <c r="G1" s="5" t="s">
         <v>20</v>
@@ -814,30 +814,30 @@
     </row>
     <row r="2" spans="1:9" s="7" customFormat="1" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B2" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D2" s="4" t="s">
         <v>30</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>32</v>
       </c>
       <c r="E2" s="13"/>
       <c r="F2" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="G2" s="4" t="s">
         <v>33</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>35</v>
       </c>
       <c r="H2" s="4"/>
       <c r="I2" s="6"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" s="11" t="s">
-        <v>37</v>
+        <v>52</v>
       </c>
       <c r="B3" s="9"/>
       <c r="C3" s="9"/>
@@ -871,7 +871,7 @@
     </row>
     <row r="5" spans="1:9" s="20" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A5" s="17" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="B5" s="21" t="s">
         <v>19</v>
@@ -890,13 +890,13 @@
         <v>19</v>
       </c>
       <c r="H5" s="21" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="I5" s="19"/>
     </row>
     <row r="6" spans="1:9" s="20" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A6" s="14" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B6" s="18" t="s">
         <v>19</v>
@@ -915,13 +915,13 @@
         <v>19</v>
       </c>
       <c r="H6" s="18" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="I6" s="19"/>
     </row>
     <row r="7" spans="1:9" s="20" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A7" s="14" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B7" s="18" t="s">
         <v>19</v>
@@ -944,7 +944,7 @@
     </row>
     <row r="8" spans="1:9" s="20" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A8" s="17" t="s">
-        <v>23</v>
+        <v>55</v>
       </c>
       <c r="B8" s="21" t="s">
         <v>19</v>
@@ -967,7 +967,7 @@
     </row>
     <row r="9" spans="1:9" s="26" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A9" s="22" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B9" s="23" t="s">
         <v>19</v>
@@ -982,7 +982,7 @@
     </row>
     <row r="10" spans="1:9" s="26" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A10" s="22" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="B10" s="23" t="s">
         <v>19</v>
@@ -995,7 +995,7 @@
       <c r="F10" s="23"/>
       <c r="G10" s="23"/>
       <c r="H10" s="23" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="I10" s="25"/>
     </row>
@@ -1058,7 +1058,7 @@
     </row>
     <row r="14" spans="1:9" s="31" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A14" s="27" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B14" s="28" t="s">
         <v>19</v>
@@ -1098,7 +1098,7 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A16" s="11" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B16" s="9"/>
       <c r="C16" s="9"/>
@@ -1132,7 +1132,7 @@
     </row>
     <row r="18" spans="1:9" s="26" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A18" s="39" t="s">
-        <v>49</v>
+        <v>56</v>
       </c>
       <c r="B18" s="40" t="s">
         <v>19</v>
@@ -1151,7 +1151,7 @@
     </row>
     <row r="19" spans="1:9" s="36" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A19" s="32" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B19" s="33"/>
       <c r="C19" s="33"/>
@@ -1168,7 +1168,7 @@
     </row>
     <row r="20" spans="1:9" s="36" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A20" s="32" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="B20" s="33"/>
       <c r="C20" s="33"/>
@@ -1181,13 +1181,13 @@
         <v>19</v>
       </c>
       <c r="H20" s="33" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="I20" s="35"/>
     </row>
     <row r="21" spans="1:9" s="36" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A21" s="32" t="s">
-        <v>47</v>
+        <v>57</v>
       </c>
       <c r="B21" s="33"/>
       <c r="C21" s="33"/>
@@ -1201,12 +1201,12 @@
       </c>
       <c r="H21" s="37"/>
       <c r="I21" s="38" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="22" spans="1:9" s="36" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A22" s="32" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B22" s="33"/>
       <c r="C22" s="33"/>
@@ -1218,12 +1218,12 @@
       <c r="G22" s="33"/>
       <c r="H22" s="33"/>
       <c r="I22" s="35" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="23" spans="1:9" s="31" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A23" s="27" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B23" s="41" t="s">
         <v>19</v>
@@ -1305,7 +1305,7 @@
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A27" s="15" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B27" s="9"/>
       <c r="C27" s="9"/>
@@ -1362,7 +1362,7 @@
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A30" s="11" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B30" s="9"/>
       <c r="C30" s="9"/>
@@ -1396,7 +1396,7 @@
     </row>
     <row r="32" spans="1:9" s="20" customFormat="1" ht="58" x14ac:dyDescent="0.35">
       <c r="A32" s="14" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B32" s="18" t="s">
         <v>19</v>
@@ -1415,7 +1415,7 @@
         <v>19</v>
       </c>
       <c r="H32" s="18" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="I32" s="19"/>
     </row>
@@ -1438,7 +1438,7 @@
     </row>
     <row r="34" spans="1:9" s="26" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A34" s="42" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="B34" s="23"/>
       <c r="C34" s="23"/>
@@ -1470,7 +1470,7 @@
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A36" s="11" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B36" s="9"/>
       <c r="C36" s="9"/>
@@ -1496,7 +1496,7 @@
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A38" s="11" t="s">
-        <v>48</v>
+        <v>60</v>
       </c>
       <c r="B38" s="9"/>
       <c r="C38" s="9"/>
@@ -1545,7 +1545,7 @@
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A41" s="11" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B41" s="9"/>
       <c r="C41" s="9"/>
@@ -1556,7 +1556,7 @@
     </row>
     <row r="42" spans="1:9" s="26" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A42" s="39" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B42" s="23"/>
       <c r="C42" s="23"/>

</xml_diff>